<commit_message>
set page size at container level
</commit_message>
<xml_diff>
--- a/samples/问题作品清单.xlsx
+++ b/samples/问题作品清单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="10300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="9700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,39 +19,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>雾霾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://ac-hf3jpeco.clouddn.com/4530e671fd9639d97702.json?1464560104218</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搞定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动画显示有问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.agoodme.com/#/preview/tid=154f1afea68395f2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>http://ac-hf3jpeco.clouddn.com/7e21406425ab0331cf6b.json?1464559603810</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>雾霾</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://ac-hf3jpeco.clouddn.com/4530e671fd9639d97702.json?1464560104218</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搞定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://ac-hf3jpeco.clouddn.com/1f0b82a68fdea955281a.json?1464579794118</t>
-  </si>
-  <si>
-    <t>动画显示有问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://ac-hf3jpeco.clouddn.com/e3989024061582aebc70.json?1464251726690</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://ac-hf3jpeco.clouddn.com/04067f66a2ef7fbe0477.json?1464579982507</t>
-  </si>
-  <si>
-    <t>http://ac-hf3jpeco.clouddn.com/e3989024061582aebc70.json?1464251726690</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>154ff30871da27f6</t>
+  </si>
+  <si>
+    <t>显示误差大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://ac-hf3jpeco.clouddn.com/9d7733f70974d624de11.json?1464688787864</t>
+  </si>
+  <si>
+    <t>很多类型不能处理，歌曲不支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1515c33054ca5d9c</t>
+  </si>
+  <si>
+    <t>图片处理错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -387,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -399,44 +431,74 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -444,8 +506,12 @@
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3" location="/preview/tid=154f1afea68395f2"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>